<commit_message>
update bsm1 cached results and figures
</commit_message>
<xml_diff>
--- a/exposan/bsm1/cached_results_figures/results/KS_test.xlsx
+++ b/exposan/bsm1/cached_results_figures/results/KS_test.xlsx
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.05398602835422232</v>
+        <v>0.06225618820524588</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04584963756494964</v>
+        <v>0.05015661212735886</v>
       </c>
     </row>
     <row r="5">
@@ -544,10 +544,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.03438120676665982</v>
+        <v>0.1402560086200876</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05072487010071204</v>
+        <v>0.05532542330078897</v>
       </c>
     </row>
     <row r="6">
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.09499349359632901</v>
+        <v>0.05565144516167653</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04381294502533838</v>
+        <v>0.03415325586226279</v>
       </c>
     </row>
     <row r="7">
@@ -576,382 +576,368 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1272344359975344</v>
+        <v>0.092486356516447</v>
       </c>
       <c r="D7" t="n">
-        <v>0.03633972673038681</v>
+        <v>0.05431935839941999</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O1</t>
-        </is>
-      </c>
+      <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Aerobic zone hydraulic retention time [hr]</t>
+          <t>ASM1 mu H [/d]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.06583453188137799</v>
+        <v>0.113268350111243</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2245333247802938</v>
+        <v>0.07991902603142018</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O3</t>
-        </is>
-      </c>
+      <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Internal recirculation rate as a fraction of influent</t>
+          <t>ASM1 K S [g COD/m3]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.04023697007054312</v>
+        <v>0.06982869571290319</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07555006735518635</v>
+        <v>0.0476068282072901</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Flat bottom circular clarifier-C1</t>
-        </is>
-      </c>
+      <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Sludge recycling as a fraction of influent</t>
+          <t>ASM1 K O H [g O2/m3]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.106122868296692</v>
+        <v>0.2456226117668187</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1281352235550709</v>
+        <v>0.09022406328026035</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Waste sludge flowrate [m3/d]</t>
+          <t>ASM1 K NO [g N/m3]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1274056571467708</v>
+        <v>0.1170995001546428</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2064596831098852</v>
+        <v>0.0829942446570622</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-A1</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>ASM1 mu H [/d]</t>
+          <t>ASM1 b H [/d]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.09334977056366002</v>
+        <v>0.1263980205724776</v>
       </c>
       <c r="D12" t="n">
-        <v>0.04931361857720187</v>
+        <v>0.05125635918553548</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K S [g COD/m3]</t>
+          <t>ASM1 mu A [/d]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.1054893500445175</v>
+        <v>0.1731300695393641</v>
       </c>
       <c r="D13" t="n">
-        <v>0.06097248059529155</v>
+        <v>0.1445963724639629</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K O H [g O2/m3]</t>
+          <t>ASM1 K NH [g N/m3]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.2379289089788371</v>
+        <v>0.1455837016491904</v>
       </c>
       <c r="D14" t="n">
-        <v>0.05019565077939573</v>
+        <v>0.1610885051993597</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K NO [g N/m3]</t>
+          <t>ASM1 K O A [g COD/m3]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.1266180398602836</v>
+        <v>0.1684508784707326</v>
       </c>
       <c r="D15" t="n">
-        <v>0.04835140162935403</v>
+        <v>0.1135631397371197</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>ASM1 b H [/d]</t>
+          <t>ASM1 b A [/d]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.07797411136223546</v>
+        <v>0.1248216619608704</v>
       </c>
       <c r="D16" t="n">
-        <v>0.08547693886714991</v>
+        <v>0.1101661432685297</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>ASM1 mu A [/d]</t>
+          <t>ASM1 eta g</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.08793918224779125</v>
+        <v>0.1415131047280781</v>
       </c>
       <c r="D17" t="n">
-        <v>0.122826993392777</v>
+        <v>0.08115318661892949</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K NH [g N/m3]</t>
+          <t>ASM1 k a [m3/g COD/d]</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.1083144990069173</v>
+        <v>0.1354770480190759</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1891718519468856</v>
+        <v>0.08178044975581542</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K O A [g COD/m3]</t>
+          <t>ASM1 k h [g X_S/g X_BH COD/d]</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.1659989041846449</v>
+        <v>0.1546527521425507</v>
       </c>
       <c r="D19" t="n">
-        <v>0.08752966835589197</v>
+        <v>0.05821327761281572</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>ASM1 b A [/d]</t>
+          <t>ASM1 K X [g X_S/g X_BH COD]</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.09001095815355113</v>
+        <v>0.06406201674132753</v>
       </c>
       <c r="D20" t="n">
-        <v>0.09086535377509783</v>
+        <v>0.04058473958396976</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>ASM1 eta g</t>
+          <t>ASM1 eta h</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.12434079857544</v>
+        <v>0.08142191537548263</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04870421451023157</v>
+        <v>0.05716240820166917</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>ASM1 k a [m3/g COD/d]</t>
+          <t>ASM1 Y H [g COD/g COD]</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.06470447229641806</v>
+        <v>0.076652931727709</v>
       </c>
       <c r="D22" t="n">
-        <v>0.05341907755468599</v>
+        <v>0.04245023644561751</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>ASM1 k h [g X_S/g X_BH COD/d]</t>
+          <t>ASM1 Y A [g COD/g N]</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.08422368330936238</v>
+        <v>0.08604124472468598</v>
       </c>
       <c r="D23" t="n">
-        <v>0.05293796908076208</v>
+        <v>0.05822142388732073</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K X [g X_S/g X_BH COD]</t>
+          <t>ASM1 f pobs</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.09504485994109993</v>
+        <v>0.07346030669154253</v>
       </c>
       <c r="D24" t="n">
-        <v>0.05851882737827956</v>
+        <v>0.1019302597439626</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n"/>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>CSTR-O1</t>
+        </is>
+      </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>ASM1 eta h</t>
+          <t>Aerobic zone hydraulic retention time [hr]</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2868981576604342</v>
+        <v>0.2506410192455428</v>
       </c>
       <c r="D25" t="n">
-        <v>0.05483032907819616</v>
+        <v>0.2291261898652199</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>ASM1 Y H [g COD/g COD]</t>
+          <t>O1 and o2 kla</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1529004862680638</v>
+        <v>0.5121369636140516</v>
       </c>
       <c r="D26" t="n">
-        <v>0.07574251074475592</v>
+        <v>0.5030813283315207</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>ASM1 Y A [g COD/g N]</t>
+          <t>Saturation DO [mg/L]</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.06556057804259982</v>
+        <v>0.2627630174297373</v>
       </c>
       <c r="D27" t="n">
-        <v>0.03055038809416897</v>
+        <v>0.2688963019986885</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n"/>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>CSTR-O3</t>
+        </is>
+      </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>ASM1 f pobs</t>
+          <t>Internal recirculation rate as a fraction of influent</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.08537086500924594</v>
+        <v>0.06799293631710748</v>
       </c>
       <c r="D28" t="n">
-        <v>0.06911925075373661</v>
+        <v>0.05458003918358037</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O1</t>
-        </is>
-      </c>
+      <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>O1 and o2 kla</t>
+          <t>O3 kla</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.1144955824943497</v>
+        <v>0.06570821402560086</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5469401501058438</v>
+        <v>0.08492491171475006</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>CSTR-O3</t>
+          <t>Flat bottom circular clarifier-C1</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>O3 kla</t>
+          <t>Sludge recycling as a fraction of influent</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.06497842613519622</v>
+        <v>0.1079805648950923</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1109917249342485</v>
+        <v>0.1674833306857941</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O1</t>
-        </is>
-      </c>
+      <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Saturation DO [mg/L]</t>
+          <t>Waste sludge flowrate [m3/d]</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.07946373536059174</v>
+        <v>0.12956071474893</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2489255244082366</v>
+        <v>0.1845742145973093</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A28"/>
+    <mergeCell ref="A7:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1025,10 +1011,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4827759917676492</v>
+        <v>0.8062248012750971</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6476190283037051</v>
+        <v>0.5451617631770604</v>
       </c>
     </row>
     <row r="5">
@@ -1039,10 +1025,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9336375505447895</v>
+        <v>0.03473006018611813</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5200446040088358</v>
+        <v>0.4203241132540868</v>
       </c>
     </row>
     <row r="6">
@@ -1053,10 +1039,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.02717639045424026</v>
+        <v>0.8961722686892706</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7017431627485078</v>
+        <v>0.9243211649889043</v>
       </c>
     </row>
     <row r="7">
@@ -1071,382 +1057,368 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.000919914098518257</v>
+        <v>0.3349649328115392</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8803118899749542</v>
+        <v>0.4433230517368963</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O1</t>
-        </is>
-      </c>
+      <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Aerobic zone hydraulic retention time [hr]</t>
+          <t>ASM1 mu H [/d]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.249342377888578</v>
+        <v>0.1404084612499558</v>
       </c>
       <c r="D8" t="n">
-        <v>1.613601286658463e-11</v>
+        <v>0.08109185701253037</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O3</t>
-        </is>
-      </c>
+      <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Internal recirculation rate as a fraction of influent</t>
+          <t>ASM1 K S [g COD/m3]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.8246804306825546</v>
+        <v>0.683263662940607</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1084214021708972</v>
+        <v>0.611270278843504</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Flat bottom circular clarifier-C1</t>
-        </is>
-      </c>
+      <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Sludge recycling as a fraction of influent</t>
+          <t>ASM1 K O H [g O2/m3]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.009436915354090426</v>
+        <v>8.256633459366999e-06</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0004874979154781315</v>
+        <v>0.03390437689712211</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Waste sludge flowrate [m3/d]</t>
+          <t>ASM1 K NO [g N/m3]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0009010616470012909</v>
+        <v>0.1172684402856004</v>
       </c>
       <c r="D11" t="n">
-        <v>8.464987274073093e-10</v>
+        <v>0.06320515193315844</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-A1</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>ASM1 mu H [/d]</t>
+          <t>ASM1 b H [/d]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.03146003282971038</v>
+        <v>0.07386994212750495</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5562421493535505</v>
+        <v>0.5172952279790757</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K S [g COD/m3]</t>
+          <t>ASM1 mu A [/d]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01005392597690209</v>
+        <v>0.004230074828731686</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2956526379872814</v>
+        <v>5.983344002405235e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K O H [g O2/m3]</t>
+          <t>ASM1 K NH [g N/m3]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4.209902567600773e-12</v>
+        <v>0.02541676946673458</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5334996201207829</v>
+        <v>4.878938813632685e-06</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K NO [g N/m3]</t>
+          <t>ASM1 K O A [g COD/m3]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.0009904549518349258</v>
+        <v>0.005866027024870765</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5813320990835954</v>
+        <v>0.003200086402620198</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>ASM1 b H [/d]</t>
+          <t>ASM1 b A [/d]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.1092960325814332</v>
+        <v>0.08008577472594217</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0483726763136748</v>
+        <v>0.004663045448409871</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>ASM1 mu A [/d]</t>
+          <t>ASM1 eta g</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.05001446046379532</v>
+        <v>0.03229832419904825</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0009547867427463956</v>
+        <v>0.07340356981168983</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K NH [g N/m3]</t>
+          <t>ASM1 k a [m3/g COD/d]</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.007557650164511875</v>
+        <v>0.04545476100032474</v>
       </c>
       <c r="D18" t="n">
-        <v>2.727168624494514e-08</v>
+        <v>0.06978419152192343</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K O A [g COD/m3]</t>
+          <t>ASM1 k h [g X_S/g X_BH COD/d]</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4.244926712904324e-06</v>
+        <v>0.01457650018623719</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04043004384731436</v>
+        <v>0.3583380859833175</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>ASM1 b A [/d]</t>
+          <t>ASM1 K X [g X_S/g X_BH COD]</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.04201552607978928</v>
+        <v>0.7781994259899252</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02994349783786826</v>
+        <v>0.7930410942192309</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>ASM1 eta g</t>
+          <t>ASM1 eta h</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.001297673369154442</v>
+        <v>0.4916495304966206</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5720635952807004</v>
+        <v>0.3802261827724651</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>ASM1 k a [m3/g COD/d]</t>
+          <t>ASM1 Y H [g COD/g COD]</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.2672887283664211</v>
+        <v>0.5684565624176354</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4540045838856271</v>
+        <v>0.7464416338162054</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>ASM1 k h [g X_S/g X_BH COD/d]</t>
+          <t>ASM1 Y A [g COD/g N]</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.06767925581738569</v>
+        <v>0.4220608792171776</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4655151751127921</v>
+        <v>0.3580958582848331</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>ASM1 K X [g X_S/g X_BH COD]</t>
+          <t>ASM1 f pobs</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.02705247522886884</v>
+        <v>0.6220596507502912</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3423608082624314</v>
+        <v>0.01110895792203313</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n"/>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>CSTR-O1</t>
+        </is>
+      </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>ASM1 eta h</t>
+          <t>Aerobic zone hydraulic retention time [hr]</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.850768069948391e-17</v>
+        <v>4.932821914471342e-06</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4212434129683369</v>
+        <v>8.509111524568462e-12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>ASM1 Y H [g COD/g COD]</t>
+          <t>O1 and o2 kla</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.068276008414209e-05</v>
+        <v>9.360553488726321e-25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1068392154158138</v>
+        <v>4.235134478122423e-57</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>ASM1 Y A [g COD/g N]</t>
+          <t>Saturation DO [mg/L]</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.2536152162812247</v>
+        <v>1.358552934530584e-06</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9663621913934246</v>
+        <v>3.989584221254844e-16</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n"/>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>CSTR-O3</t>
+        </is>
+      </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>ASM1 f pobs</t>
+          <t>Internal recirculation rate as a fraction of influent</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.06173212253816688</v>
+        <v>0.7141986555968359</v>
       </c>
       <c r="D28" t="n">
-        <v>0.1734038061194453</v>
+        <v>0.4372178424932672</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O1</t>
-        </is>
-      </c>
+      <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>O1 and o2 kla</t>
+          <t>O3 kla</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.003942509116430786</v>
+        <v>0.7517594452307359</v>
       </c>
       <c r="D29" t="n">
-        <v>4.542354257214241e-69</v>
+        <v>0.05380778794020067</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>CSTR-O3</t>
+          <t>Flat bottom circular clarifier-C1</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>O3 kla</t>
+          <t>Sludge recycling as a fraction of influent</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.2628592379621416</v>
+        <v>0.1781934317256087</v>
       </c>
       <c r="D30" t="n">
-        <v>0.003856470673352684</v>
+        <v>1.712805685741369e-06</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>CSTR-O1</t>
-        </is>
-      </c>
+      <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Saturation DO [mg/L]</t>
+          <t>Waste sludge flowrate [m3/d]</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.09782306982736146</v>
+        <v>0.06260109546839047</v>
       </c>
       <c r="D31" t="n">
-        <v>4.492040187894263e-14</v>
+        <v>8.543660839223266e-08</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A28"/>
+    <mergeCell ref="A7:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>